<commit_message>
can print that weird invoice
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE218259-2474-42F4-B8D1-570C79D7F8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3530F46D-A0A1-41E2-BC8D-9351C11C0F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="3765" windowWidth="19035" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
+    <workbookView xWindow="9315" yWindow="3045" windowWidth="19035" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Vendors</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>UPS</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -426,7 +423,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,12 +479,6 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>12.43</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed beacon scanning by removing sample text
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7404A0FD-57D4-4A15-84EB-277C3713A33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED04E597-217B-4BE9-AB86-6836C77CEED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
+    <workbookView xWindow="5985" yWindow="3495" windowWidth="19020" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Vendors</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Garlock Chicago Inc.</t>
+  </si>
+  <si>
+    <t>HUB International Midwest Limited</t>
+  </si>
+  <si>
+    <t>Salvi Salvi &amp; Wifler</t>
+  </si>
+  <si>
+    <t>Hernandez Lawn Service</t>
+  </si>
+  <si>
+    <t>ComCast Business</t>
   </si>
 </sst>
 </file>
@@ -444,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9267CA-59CB-45E5-B346-87C338D47B3D}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="I1">
-        <v>33026</v>
+        <v>33085</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -492,25 +504,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>471.04</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
@@ -518,37 +533,72 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>148.16999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
monthly bill payment plus improved mail
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2013867-BA3F-4440-8AD7-1274554D5CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F628AB-5A6D-4C77-9C12-A389CEBDE3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5985" yWindow="3495" windowWidth="19020" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Vendors</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>ComCast Business</t>
-  </si>
-  <si>
-    <t>00007RW518363</t>
   </si>
 </sst>
 </file>
@@ -462,7 +459,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,6 +516,12 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>278.62</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -532,6 +535,9 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
       <c r="G7" t="s">
         <v>13</v>
       </c>
@@ -591,15 +597,6 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16">
-        <v>20.100000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added an abs path
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9686EC0-F560-41DD-AFA4-61A5770666E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65E0738-402E-40DA-AC05-53489E95A61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9345" yWindow="3360" windowWidth="19020" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
+    <workbookView xWindow="390" yWindow="1275" windowWidth="19020" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Vendors</t>
   </si>
@@ -459,7 +459,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="I1">
-        <v>33121</v>
+        <v>33133</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -506,12 +506,6 @@
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>471.04</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -543,12 +537,6 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8">
-        <v>50.43</v>
-      </c>
       <c r="G8" t="s">
         <v>13</v>
       </c>
@@ -575,16 +563,16 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>187.45</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>343.65</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cut out unnecessary api calls, added logic for blank subjects on emails
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65E0738-402E-40DA-AC05-53489E95A61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAD1566-ADB9-4FE2-A716-A9BA208BEA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="1275" windowWidth="19020" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
+    <workbookView xWindow="3000" yWindow="3645" windowWidth="19020" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Vendors</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>ComCast Business</t>
+  </si>
+  <si>
+    <t>Safety Check Inc.</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9267CA-59CB-45E5-B346-87C338D47B3D}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +497,7 @@
         <v>14</v>
       </c>
       <c r="I1">
-        <v>33133</v>
+        <v>33139</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -529,6 +532,15 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>6649</v>
+      </c>
+      <c r="D7">
+        <v>1230</v>
+      </c>
       <c r="G7" t="s">
         <v>13</v>
       </c>
@@ -558,6 +570,12 @@
       <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>145.80000000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -566,26 +584,29 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
+      <c r="C13">
+        <v>13727</v>
+      </c>
       <c r="D13">
-        <v>343.65</v>
+        <v>2205</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
         <v>13</v>
@@ -593,6 +614,14 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
switched from ghostscript to sumatra
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAD1566-ADB9-4FE2-A716-A9BA208BEA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103AA60C-3024-459F-85B7-8772550FEECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="3645" windowWidth="19020" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Vendors</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>ComCast Business</t>
-  </si>
-  <si>
-    <t>Safety Check Inc.</t>
   </si>
 </sst>
 </file>
@@ -459,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9267CA-59CB-45E5-B346-87C338D47B3D}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,29 +581,20 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>13727</v>
-      </c>
-      <c r="D13">
-        <v>2205</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
         <v>13</v>
@@ -614,14 +602,6 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
connection broken with scan
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\python-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CC56F2-21C1-4766-B7E2-2C89731FEF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7F6612-F9C2-4C66-973A-D8763C83D59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
+    <workbookView xWindow="4560" yWindow="4680" windowWidth="23190" windowHeight="10920" xr2:uid="{8140579D-6B44-493B-BE20-36C75E9AAFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Vendors</t>
   </si>
@@ -484,7 +484,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +519,7 @@
         <v>14</v>
       </c>
       <c r="I1">
-        <v>33514</v>
+        <v>33557</v>
       </c>
       <c r="J1" t="s">
         <v>30</v>
@@ -537,12 +537,6 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>4670.8999999999996</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -558,6 +552,12 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>87836.9</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -591,15 +591,6 @@
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>6838</v>
-      </c>
-      <c r="D12">
-        <v>1512.5</v>
-      </c>
       <c r="G12" t="s">
         <v>13</v>
       </c>
@@ -630,8 +621,8 @@
         <v>15</v>
       </c>
       <c r="I16">
-        <f>222.9+192.89+236.19</f>
-        <v>651.98</v>
+        <f>156.05+175.85+262.61</f>
+        <v>594.51</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>